<commit_message>
Modifications car 2021-01-12 manque aussi
</commit_message>
<xml_diff>
--- a/Final_results/BDF_excel_2020.xlsx
+++ b/Final_results/BDF_excel_2020.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="399">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -929,20 +929,13 @@
     <t xml:space="preserve">2021-01-12</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, giving a speech about the economic outlook of France. Today is 12 January 2021. You will be provided with a document with information about the current state and recent past of the French economy. Using ONLY the information in that document and information that was available on or before 12 January 2021, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the fourth quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
+    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, and you are giving a speech about the economic outlook of France. Today is 12 January 2021. Using ONLY information that was available on or before 12 January 2021, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the fourth quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
 &lt;forecast&gt; (&lt;confidence&gt;)
 Example: +0.3 (80)
 Do NOT use any information published after 12 January 2021.</t>
   </si>
   <si>
-    <t xml:space="preserve">
--2.5 (80)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.5 (80)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.7 (90)</t>
+    <t xml:space="preserve">-2.5 (75)</t>
   </si>
   <si>
     <t xml:space="preserve">-4.0 (85)</t>
@@ -9010,7 +9003,7 @@
         <v>-2.5</v>
       </c>
       <c r="D73" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E73" t="s">
         <v>234</v>
@@ -9019,55 +9012,55 @@
         <v>-2.5</v>
       </c>
       <c r="G73" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H73" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I73" t="n">
         <v>-2.5</v>
       </c>
       <c r="J73" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="K73" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L73" t="n">
-        <v>-2.7</v>
+        <v>-4</v>
       </c>
       <c r="M73" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="N73" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="O73" t="n">
-        <v>-2.7</v>
+        <v>-4</v>
       </c>
       <c r="P73" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="Q73" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="R73" t="n">
         <v>-4</v>
       </c>
       <c r="S73" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="T73" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="U73" t="n">
         <v>-4</v>
       </c>
       <c r="V73" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="W73" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="X73" t="n">
         <v>-4</v>
@@ -9076,7 +9069,7 @@
         <v>85</v>
       </c>
       <c r="Z73" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AA73" t="n">
         <v>-4</v>
@@ -9085,7 +9078,7 @@
         <v>85</v>
       </c>
       <c r="AC73" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AD73" t="n">
         <v>-4</v>
@@ -9094,15 +9087,15 @@
         <v>85</v>
       </c>
       <c r="AF73" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B74" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C74" t="n">
         <v>0.2</v>
@@ -9111,7 +9104,7 @@
         <v>55</v>
       </c>
       <c r="E74" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F74" t="n">
         <v>0.2</v>
@@ -9120,7 +9113,7 @@
         <v>55</v>
       </c>
       <c r="H74" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I74" t="n">
         <v>0.2</v>
@@ -9129,7 +9122,7 @@
         <v>55</v>
       </c>
       <c r="K74" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L74" t="n">
         <v>0.2</v>
@@ -9174,7 +9167,7 @@
         <v>60</v>
       </c>
       <c r="Z74" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AA74" t="n">
         <v>-0.2</v>
@@ -9183,7 +9176,7 @@
         <v>60</v>
       </c>
       <c r="AC74" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AD74" t="n">
         <v>-0.2</v>
@@ -9192,15 +9185,15 @@
         <v>60</v>
       </c>
       <c r="AF74" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B75" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C75" t="n">
         <v>0.4</v>
@@ -9254,7 +9247,7 @@
         <v>65</v>
       </c>
       <c r="T75" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="U75" t="n">
         <v>0.5</v>
@@ -9263,7 +9256,7 @@
         <v>65</v>
       </c>
       <c r="W75" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="X75" t="n">
         <v>0.4</v>
@@ -9295,10 +9288,10 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B76" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C76" t="n">
         <v>0.1</v>
@@ -9393,10 +9386,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B77" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C77" t="n">
         <v>1.5</v>
@@ -9405,7 +9398,7 @@
         <v>75</v>
       </c>
       <c r="E77" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F77" t="n">
         <v>1.5</v>
@@ -9414,7 +9407,7 @@
         <v>75</v>
       </c>
       <c r="H77" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I77" t="n">
         <v>1.5</v>
@@ -9423,7 +9416,7 @@
         <v>75</v>
       </c>
       <c r="K77" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L77" t="n">
         <v>0.8</v>
@@ -9432,7 +9425,7 @@
         <v>75</v>
       </c>
       <c r="N77" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="O77" t="n">
         <v>0.8</v>
@@ -9441,7 +9434,7 @@
         <v>75</v>
       </c>
       <c r="Q77" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="R77" t="n">
         <v>0.5</v>
@@ -9450,7 +9443,7 @@
         <v>75</v>
       </c>
       <c r="T77" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="U77" t="n">
         <v>0.5</v>
@@ -9459,7 +9452,7 @@
         <v>75</v>
       </c>
       <c r="W77" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="X77" t="n">
         <v>0.5</v>
@@ -9491,10 +9484,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B78" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C78" t="n">
         <v>1</v>
@@ -9503,7 +9496,7 @@
         <v>90</v>
       </c>
       <c r="E78" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F78" t="n">
         <v>1</v>
@@ -9512,7 +9505,7 @@
         <v>90</v>
       </c>
       <c r="H78" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I78" t="n">
         <v>1</v>
@@ -9521,7 +9514,7 @@
         <v>90</v>
       </c>
       <c r="K78" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="L78" t="n">
         <v>0.7</v>
@@ -9530,7 +9523,7 @@
         <v>85</v>
       </c>
       <c r="N78" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O78" t="n">
         <v>0.7</v>
@@ -9539,7 +9532,7 @@
         <v>85</v>
       </c>
       <c r="Q78" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="R78" t="n">
         <v>0.8</v>
@@ -9548,7 +9541,7 @@
         <v>90</v>
       </c>
       <c r="T78" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="U78" t="n">
         <v>0.8</v>
@@ -9557,7 +9550,7 @@
         <v>90</v>
       </c>
       <c r="W78" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="X78" t="n">
         <v>0.8</v>
@@ -9566,7 +9559,7 @@
         <v>85</v>
       </c>
       <c r="Z78" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AA78" t="n">
         <v>0.8</v>
@@ -9575,7 +9568,7 @@
         <v>85</v>
       </c>
       <c r="AC78" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AD78" t="n">
         <v>0.8</v>
@@ -9584,15 +9577,15 @@
         <v>85</v>
       </c>
       <c r="AF78" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B79" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C79" t="n">
         <v>0.9</v>
@@ -9601,7 +9594,7 @@
         <v>90</v>
       </c>
       <c r="E79" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F79" t="n">
         <v>0.9</v>
@@ -9610,7 +9603,7 @@
         <v>90</v>
       </c>
       <c r="H79" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I79" t="n">
         <v>0.9</v>
@@ -9619,7 +9612,7 @@
         <v>90</v>
       </c>
       <c r="K79" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L79" t="n">
         <v>0.8</v>
@@ -9628,7 +9621,7 @@
         <v>90</v>
       </c>
       <c r="N79" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O79" t="n">
         <v>0.8</v>
@@ -9637,7 +9630,7 @@
         <v>90</v>
       </c>
       <c r="Q79" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="R79" t="n">
         <v>0.9</v>
@@ -9646,7 +9639,7 @@
         <v>90</v>
       </c>
       <c r="T79" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="U79" t="n">
         <v>0.9</v>
@@ -9655,7 +9648,7 @@
         <v>90</v>
       </c>
       <c r="W79" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="X79" t="n">
         <v>0.8</v>
@@ -9664,7 +9657,7 @@
         <v>85</v>
       </c>
       <c r="Z79" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AA79" t="n">
         <v>0.8</v>
@@ -9673,7 +9666,7 @@
         <v>85</v>
       </c>
       <c r="AC79" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AD79" t="n">
         <v>0.8</v>
@@ -9682,15 +9675,15 @@
         <v>85</v>
       </c>
       <c r="AF79" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B80" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C80" t="n">
         <v>2.3</v>
@@ -9699,7 +9692,7 @@
         <v>90</v>
       </c>
       <c r="E80" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F80" t="n">
         <v>2.3</v>
@@ -9708,7 +9701,7 @@
         <v>90</v>
       </c>
       <c r="H80" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I80" t="n">
         <v>2.3</v>
@@ -9717,7 +9710,7 @@
         <v>90</v>
       </c>
       <c r="K80" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L80" t="n">
         <v>2.5</v>
@@ -9726,7 +9719,7 @@
         <v>70</v>
       </c>
       <c r="N80" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="O80" t="n">
         <v>2.5</v>
@@ -9735,7 +9728,7 @@
         <v>70</v>
       </c>
       <c r="Q80" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="R80" t="n">
         <v>2.5</v>
@@ -9744,7 +9737,7 @@
         <v>85</v>
       </c>
       <c r="T80" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="U80" t="n">
         <v>2.5</v>
@@ -9753,7 +9746,7 @@
         <v>85</v>
       </c>
       <c r="W80" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="X80" t="n">
         <v>1.1</v>
@@ -9762,7 +9755,7 @@
         <v>85</v>
       </c>
       <c r="Z80" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AA80" t="n">
         <v>1.1</v>
@@ -9771,7 +9764,7 @@
         <v>85</v>
       </c>
       <c r="AC80" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AD80" t="n">
         <v>1.1</v>
@@ -9780,15 +9773,15 @@
         <v>85</v>
       </c>
       <c r="AF80" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B81" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C81" t="n">
         <v>2.3</v>
@@ -9797,7 +9790,7 @@
         <v>75</v>
       </c>
       <c r="E81" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F81" t="n">
         <v>2.3</v>
@@ -9806,7 +9799,7 @@
         <v>75</v>
       </c>
       <c r="H81" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I81" t="n">
         <v>2.3</v>
@@ -9815,7 +9808,7 @@
         <v>75</v>
       </c>
       <c r="K81" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L81" t="n">
         <v>2.3</v>
@@ -9824,7 +9817,7 @@
         <v>90</v>
       </c>
       <c r="N81" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="O81" t="n">
         <v>2.3</v>
@@ -9833,7 +9826,7 @@
         <v>90</v>
       </c>
       <c r="Q81" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="R81" t="n">
         <v>2.3</v>
@@ -9842,7 +9835,7 @@
         <v>90</v>
       </c>
       <c r="T81" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="U81" t="n">
         <v>2.3</v>
@@ -9851,7 +9844,7 @@
         <v>90</v>
       </c>
       <c r="W81" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="X81" t="n">
         <v>2.3</v>
@@ -9860,7 +9853,7 @@
         <v>90</v>
       </c>
       <c r="Z81" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AA81" t="n">
         <v>2.3</v>
@@ -9869,7 +9862,7 @@
         <v>90</v>
       </c>
       <c r="AC81" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AD81" t="n">
         <v>2.3</v>
@@ -9878,15 +9871,15 @@
         <v>90</v>
       </c>
       <c r="AF81" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B82" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C82" t="n">
         <v>2.3</v>
@@ -9895,7 +9888,7 @@
         <v>85</v>
       </c>
       <c r="E82" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F82" t="n">
         <v>2.3</v>
@@ -9904,7 +9897,7 @@
         <v>85</v>
       </c>
       <c r="H82" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I82" t="n">
         <v>2.3</v>
@@ -9913,7 +9906,7 @@
         <v>85</v>
       </c>
       <c r="K82" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L82" t="n">
         <v>2.3</v>
@@ -9922,7 +9915,7 @@
         <v>85</v>
       </c>
       <c r="N82" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="O82" t="n">
         <v>2.3</v>
@@ -9931,7 +9924,7 @@
         <v>85</v>
       </c>
       <c r="Q82" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="R82" t="n">
         <v>2.3</v>
@@ -9940,7 +9933,7 @@
         <v>75</v>
       </c>
       <c r="T82" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="U82" t="n">
         <v>2.3</v>
@@ -9949,7 +9942,7 @@
         <v>75</v>
       </c>
       <c r="W82" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="X82" t="n">
         <v>2.1</v>
@@ -9958,7 +9951,7 @@
         <v>85</v>
       </c>
       <c r="Z82" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="AA82" t="n">
         <v>2.1</v>
@@ -9967,7 +9960,7 @@
         <v>85</v>
       </c>
       <c r="AC82" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="AD82" t="n">
         <v>2.1</v>
@@ -9976,15 +9969,15 @@
         <v>85</v>
       </c>
       <c r="AF82" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B83" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C83" t="n">
         <v>0.7</v>
@@ -9993,7 +9986,7 @@
         <v>75</v>
       </c>
       <c r="E83" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F83" t="n">
         <v>0.7</v>
@@ -10002,7 +9995,7 @@
         <v>75</v>
       </c>
       <c r="H83" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I83" t="n">
         <v>0.7</v>
@@ -10011,7 +10004,7 @@
         <v>75</v>
       </c>
       <c r="K83" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L83" t="n">
         <v>0.6</v>
@@ -10020,7 +10013,7 @@
         <v>80</v>
       </c>
       <c r="N83" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="O83" t="n">
         <v>0.6</v>
@@ -10029,7 +10022,7 @@
         <v>80</v>
       </c>
       <c r="Q83" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="R83" t="n">
         <v>0.7</v>
@@ -10038,7 +10031,7 @@
         <v>75</v>
       </c>
       <c r="T83" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="U83" t="n">
         <v>0.7</v>
@@ -10047,7 +10040,7 @@
         <v>75</v>
       </c>
       <c r="W83" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="X83" t="n">
         <v>0.8</v>
@@ -10056,7 +10049,7 @@
         <v>75</v>
       </c>
       <c r="Z83" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AA83" t="n">
         <v>0.8</v>
@@ -10065,7 +10058,7 @@
         <v>75</v>
       </c>
       <c r="AC83" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AD83" t="n">
         <v>0.8</v>
@@ -10074,15 +10067,15 @@
         <v>75</v>
       </c>
       <c r="AF83" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B84" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C84" t="n">
         <v>0.6</v>
@@ -10091,7 +10084,7 @@
         <v>75</v>
       </c>
       <c r="E84" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F84" t="n">
         <v>0.6</v>
@@ -10100,7 +10093,7 @@
         <v>75</v>
       </c>
       <c r="H84" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I84" t="n">
         <v>0.6</v>
@@ -10109,7 +10102,7 @@
         <v>75</v>
       </c>
       <c r="K84" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L84" t="n">
         <v>0.7</v>
@@ -10118,7 +10111,7 @@
         <v>80</v>
       </c>
       <c r="N84" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="O84" t="n">
         <v>0.7</v>
@@ -10127,7 +10120,7 @@
         <v>80</v>
       </c>
       <c r="Q84" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="R84" t="n">
         <v>0.8</v>
@@ -10136,7 +10129,7 @@
         <v>80</v>
       </c>
       <c r="T84" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="U84" t="n">
         <v>0.8</v>
@@ -10145,7 +10138,7 @@
         <v>80</v>
       </c>
       <c r="W84" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="X84" t="n">
         <v>0.7</v>
@@ -10154,7 +10147,7 @@
         <v>75</v>
       </c>
       <c r="Z84" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AA84" t="n">
         <v>0.7</v>
@@ -10163,7 +10156,7 @@
         <v>75</v>
       </c>
       <c r="AC84" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AD84" t="n">
         <v>0.7</v>
@@ -10172,15 +10165,15 @@
         <v>75</v>
       </c>
       <c r="AF84" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B85" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C85" t="n">
         <v>0.6</v>
@@ -10189,7 +10182,7 @@
         <v>85</v>
       </c>
       <c r="E85" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F85" t="n">
         <v>0.6</v>
@@ -10198,7 +10191,7 @@
         <v>85</v>
       </c>
       <c r="H85" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I85" t="n">
         <v>0.6</v>
@@ -10207,7 +10200,7 @@
         <v>85</v>
       </c>
       <c r="K85" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="L85" t="n">
         <v>0.5</v>
@@ -10234,7 +10227,7 @@
         <v>85</v>
       </c>
       <c r="T85" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="U85" t="n">
         <v>0.6</v>
@@ -10243,7 +10236,7 @@
         <v>85</v>
       </c>
       <c r="W85" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="X85" t="n">
         <v>0.6</v>
@@ -10275,10 +10268,10 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B86" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C86" t="n">
         <v>0.3</v>
@@ -10373,10 +10366,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B87" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C87" t="n">
         <v>0.3</v>
@@ -10385,7 +10378,7 @@
         <v>50</v>
       </c>
       <c r="E87" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F87" t="n">
         <v>0.3</v>
@@ -10394,7 +10387,7 @@
         <v>50</v>
       </c>
       <c r="H87" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I87" t="n">
         <v>0.3</v>
@@ -10403,7 +10396,7 @@
         <v>50</v>
       </c>
       <c r="K87" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="L87" t="n">
         <v>0.3</v>
@@ -10412,7 +10405,7 @@
         <v>50</v>
       </c>
       <c r="N87" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="O87" t="n">
         <v>0.3</v>
@@ -10421,7 +10414,7 @@
         <v>50</v>
       </c>
       <c r="Q87" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="R87" t="n">
         <v>0.3</v>
@@ -10430,7 +10423,7 @@
         <v>60</v>
       </c>
       <c r="T87" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="U87" t="n">
         <v>-0.2</v>
@@ -10439,7 +10432,7 @@
         <v>40</v>
       </c>
       <c r="W87" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="X87" t="n">
         <v>0.2</v>
@@ -10448,7 +10441,7 @@
         <v>40</v>
       </c>
       <c r="Z87" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="AA87" t="n">
         <v>0.2</v>
@@ -10457,7 +10450,7 @@
         <v>40</v>
       </c>
       <c r="AC87" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="AD87" t="n">
         <v>0.2</v>
@@ -10466,15 +10459,15 @@
         <v>40</v>
       </c>
       <c r="AF87" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B88" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C88" t="n">
         <v>0.3</v>
@@ -10528,7 +10521,7 @@
         <v>50</v>
       </c>
       <c r="T88" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="U88" t="n">
         <v>0.2</v>
@@ -10537,7 +10530,7 @@
         <v>50</v>
       </c>
       <c r="W88" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="X88" t="n">
         <v>0.3</v>
@@ -10569,10 +10562,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B89" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C89" t="n">
         <v>0.2</v>
@@ -10608,7 +10601,7 @@
         <v>60</v>
       </c>
       <c r="N89" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="O89" t="n">
         <v>0.3</v>
@@ -10617,7 +10610,7 @@
         <v>60</v>
       </c>
       <c r="Q89" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="R89" t="n">
         <v>0.2</v>
@@ -10667,10 +10660,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B90" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C90" t="n">
         <v>0.2</v>
@@ -10765,10 +10758,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B91" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C91" t="n">
         <v>0.3</v>
@@ -10863,10 +10856,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B92" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C92" t="n">
         <v>0.3</v>
@@ -10961,10 +10954,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B93" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C93" t="n">
         <v>0.2</v>
@@ -10973,7 +10966,7 @@
         <v>55</v>
       </c>
       <c r="E93" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F93" t="n">
         <v>0.2</v>
@@ -10982,7 +10975,7 @@
         <v>55</v>
       </c>
       <c r="H93" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I93" t="n">
         <v>0.2</v>
@@ -10991,7 +10984,7 @@
         <v>55</v>
       </c>
       <c r="K93" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L93" t="n">
         <v>0.3</v>
@@ -11036,7 +11029,7 @@
         <v>60</v>
       </c>
       <c r="Z93" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AA93" t="n">
         <v>0.3</v>
@@ -11045,7 +11038,7 @@
         <v>60</v>
       </c>
       <c r="AC93" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AD93" t="n">
         <v>0.3</v>
@@ -11054,15 +11047,15 @@
         <v>60</v>
       </c>
       <c r="AF93" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B94" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C94" t="n">
         <v>0.3</v>
@@ -11157,10 +11150,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B95" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C95" t="n">
         <v>0.1</v>
@@ -11196,7 +11189,7 @@
         <v>65</v>
       </c>
       <c r="N95" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="O95" t="n">
         <v>-0.1</v>
@@ -11205,7 +11198,7 @@
         <v>65</v>
       </c>
       <c r="Q95" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="R95" t="n">
         <v>0.1</v>
@@ -11232,7 +11225,7 @@
         <v>60</v>
       </c>
       <c r="Z95" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AA95" t="n">
         <v>-0.1</v>
@@ -11241,7 +11234,7 @@
         <v>55</v>
       </c>
       <c r="AC95" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="AD95" t="n">
         <v>-0.1</v>
@@ -11250,52 +11243,52 @@
         <v>55</v>
       </c>
       <c r="AF95" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
+        <v>313</v>
+      </c>
+      <c r="B96" t="s">
+        <v>314</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D96" t="n">
+        <v>70</v>
+      </c>
+      <c r="E96" t="s">
         <v>315</v>
       </c>
-      <c r="B96" t="s">
+      <c r="F96" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G96" t="n">
+        <v>70</v>
+      </c>
+      <c r="H96" t="s">
+        <v>315</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J96" t="n">
+        <v>70</v>
+      </c>
+      <c r="K96" t="s">
+        <v>315</v>
+      </c>
+      <c r="L96" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M96" t="n">
+        <v>75</v>
+      </c>
+      <c r="N96" t="s">
         <v>316</v>
       </c>
-      <c r="C96" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D96" t="n">
-        <v>70</v>
-      </c>
-      <c r="E96" t="s">
-        <v>317</v>
-      </c>
-      <c r="F96" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G96" t="n">
-        <v>70</v>
-      </c>
-      <c r="H96" t="s">
-        <v>317</v>
-      </c>
-      <c r="I96" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="J96" t="n">
-        <v>70</v>
-      </c>
-      <c r="K96" t="s">
-        <v>317</v>
-      </c>
-      <c r="L96" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M96" t="n">
-        <v>75</v>
-      </c>
-      <c r="N96" t="s">
-        <v>318</v>
-      </c>
       <c r="O96" t="n">
         <v>0.1</v>
       </c>
@@ -11303,7 +11296,7 @@
         <v>75</v>
       </c>
       <c r="Q96" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="R96" t="n">
         <v>0.1</v>
@@ -11330,7 +11323,7 @@
         <v>70</v>
       </c>
       <c r="Z96" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AA96" t="n">
         <v>0.1</v>
@@ -11339,7 +11332,7 @@
         <v>70</v>
       </c>
       <c r="AC96" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AD96" t="n">
         <v>0.1</v>
@@ -11348,88 +11341,88 @@
         <v>70</v>
       </c>
       <c r="AF96" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
+        <v>317</v>
+      </c>
+      <c r="B97" t="s">
+        <v>318</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D97" t="n">
+        <v>70</v>
+      </c>
+      <c r="E97" t="s">
+        <v>315</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G97" t="n">
+        <v>70</v>
+      </c>
+      <c r="H97" t="s">
+        <v>315</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J97" t="n">
+        <v>70</v>
+      </c>
+      <c r="K97" t="s">
+        <v>315</v>
+      </c>
+      <c r="L97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M97" t="n">
+        <v>75</v>
+      </c>
+      <c r="N97" t="s">
+        <v>316</v>
+      </c>
+      <c r="O97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P97" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>316</v>
+      </c>
+      <c r="R97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S97" t="n">
+        <v>75</v>
+      </c>
+      <c r="T97" t="s">
+        <v>316</v>
+      </c>
+      <c r="U97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="V97" t="n">
+        <v>75</v>
+      </c>
+      <c r="W97" t="s">
+        <v>316</v>
+      </c>
+      <c r="X97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Y97" t="n">
+        <v>85</v>
+      </c>
+      <c r="Z97" t="s">
         <v>319</v>
       </c>
-      <c r="B97" t="s">
-        <v>320</v>
-      </c>
-      <c r="C97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D97" t="n">
-        <v>70</v>
-      </c>
-      <c r="E97" t="s">
-        <v>317</v>
-      </c>
-      <c r="F97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G97" t="n">
-        <v>70</v>
-      </c>
-      <c r="H97" t="s">
-        <v>317</v>
-      </c>
-      <c r="I97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="J97" t="n">
-        <v>70</v>
-      </c>
-      <c r="K97" t="s">
-        <v>317</v>
-      </c>
-      <c r="L97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M97" t="n">
-        <v>75</v>
-      </c>
-      <c r="N97" t="s">
-        <v>318</v>
-      </c>
-      <c r="O97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="P97" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>318</v>
-      </c>
-      <c r="R97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="S97" t="n">
-        <v>75</v>
-      </c>
-      <c r="T97" t="s">
-        <v>318</v>
-      </c>
-      <c r="U97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="V97" t="n">
-        <v>75</v>
-      </c>
-      <c r="W97" t="s">
-        <v>318</v>
-      </c>
-      <c r="X97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="Y97" t="n">
-        <v>85</v>
-      </c>
-      <c r="Z97" t="s">
-        <v>321</v>
-      </c>
       <c r="AA97" t="n">
         <v>0.1</v>
       </c>
@@ -11437,7 +11430,7 @@
         <v>85</v>
       </c>
       <c r="AC97" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AD97" t="n">
         <v>0.1</v>
@@ -11446,15 +11439,15 @@
         <v>85</v>
       </c>
       <c r="AF97" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B98" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C98" t="n">
         <v>0.1</v>
@@ -11508,7 +11501,7 @@
         <v>70</v>
       </c>
       <c r="T98" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="U98" t="n">
         <v>0.1</v>
@@ -11517,7 +11510,7 @@
         <v>70</v>
       </c>
       <c r="W98" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="X98" t="n">
         <v>0.1</v>
@@ -11549,10 +11542,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B99" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C99" t="n">
         <v>0.1</v>
@@ -11561,7 +11554,7 @@
         <v>75</v>
       </c>
       <c r="E99" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F99" t="n">
         <v>0.1</v>
@@ -11570,7 +11563,7 @@
         <v>75</v>
       </c>
       <c r="H99" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I99" t="n">
         <v>0.1</v>
@@ -11579,7 +11572,7 @@
         <v>75</v>
       </c>
       <c r="K99" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L99" t="n">
         <v>0.1</v>
@@ -11588,7 +11581,7 @@
         <v>70</v>
       </c>
       <c r="N99" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O99" t="n">
         <v>0.1</v>
@@ -11597,7 +11590,7 @@
         <v>70</v>
       </c>
       <c r="Q99" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R99" t="n">
         <v>0.2</v>
@@ -11624,7 +11617,7 @@
         <v>75</v>
       </c>
       <c r="Z99" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AA99" t="n">
         <v>0.1</v>
@@ -11633,7 +11626,7 @@
         <v>75</v>
       </c>
       <c r="AC99" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AD99" t="n">
         <v>0.1</v>
@@ -11642,15 +11635,15 @@
         <v>75</v>
       </c>
       <c r="AF99" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B100" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C100" t="n">
         <v>0.2</v>
@@ -11722,7 +11715,7 @@
         <v>80</v>
       </c>
       <c r="Z100" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AA100" t="n">
         <v>0.1</v>
@@ -11731,7 +11724,7 @@
         <v>80</v>
       </c>
       <c r="AC100" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AD100" t="n">
         <v>0.1</v>
@@ -11740,15 +11733,15 @@
         <v>80</v>
       </c>
       <c r="AF100" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B101" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C101" t="n">
         <v>0.1</v>
@@ -11784,7 +11777,7 @@
         <v>75</v>
       </c>
       <c r="N101" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O101" t="n">
         <v>0.1</v>
@@ -11793,7 +11786,7 @@
         <v>75</v>
       </c>
       <c r="Q101" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="R101" t="n">
         <v>0.1</v>
@@ -11843,10 +11836,10 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B102" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C102" t="n">
         <v>0.1</v>
@@ -11882,7 +11875,7 @@
         <v>75</v>
       </c>
       <c r="N102" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O102" t="n">
         <v>0.1</v>
@@ -11891,7 +11884,7 @@
         <v>75</v>
       </c>
       <c r="Q102" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="R102" t="n">
         <v>0.1</v>
@@ -11900,7 +11893,7 @@
         <v>80</v>
       </c>
       <c r="T102" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="U102" t="n">
         <v>0.1</v>
@@ -11909,7 +11902,7 @@
         <v>80</v>
       </c>
       <c r="W102" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="X102" t="n">
         <v>0.1</v>
@@ -11918,7 +11911,7 @@
         <v>75</v>
       </c>
       <c r="Z102" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AA102" t="n">
         <v>0.1</v>
@@ -11927,7 +11920,7 @@
         <v>75</v>
       </c>
       <c r="AC102" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AD102" t="n">
         <v>0.1</v>
@@ -11936,15 +11929,15 @@
         <v>75</v>
       </c>
       <c r="AF102" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B103" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C103" t="n">
         <v>0.1</v>
@@ -11953,7 +11946,7 @@
         <v>85</v>
       </c>
       <c r="E103" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F103" t="n">
         <v>0.1</v>
@@ -11962,7 +11955,7 @@
         <v>85</v>
       </c>
       <c r="H103" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I103" t="n">
         <v>0.1</v>
@@ -11971,7 +11964,7 @@
         <v>85</v>
       </c>
       <c r="K103" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L103" t="n">
         <v>0.1</v>
@@ -11980,7 +11973,7 @@
         <v>85</v>
       </c>
       <c r="N103" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="O103" t="n">
         <v>0.1</v>
@@ -11989,7 +11982,7 @@
         <v>85</v>
       </c>
       <c r="Q103" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="R103" t="n">
         <v>0.1</v>
@@ -11998,7 +11991,7 @@
         <v>75</v>
       </c>
       <c r="T103" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="U103" t="n">
         <v>0.1</v>
@@ -12007,7 +12000,7 @@
         <v>75</v>
       </c>
       <c r="W103" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="X103" t="n">
         <v>0.1</v>
@@ -12016,7 +12009,7 @@
         <v>75</v>
       </c>
       <c r="Z103" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AA103" t="n">
         <v>0.1</v>
@@ -12025,7 +12018,7 @@
         <v>75</v>
       </c>
       <c r="AC103" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AD103" t="n">
         <v>0.1</v>
@@ -12034,15 +12027,15 @@
         <v>75</v>
       </c>
       <c r="AF103" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B104" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C104" t="n">
         <v>0.1</v>
@@ -12051,7 +12044,7 @@
         <v>70</v>
       </c>
       <c r="E104" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F104" t="n">
         <v>0.1</v>
@@ -12060,7 +12053,7 @@
         <v>70</v>
       </c>
       <c r="H104" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I104" t="n">
         <v>0.1</v>
@@ -12069,7 +12062,7 @@
         <v>70</v>
       </c>
       <c r="K104" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L104" t="n">
         <v>0.1</v>
@@ -12096,7 +12089,7 @@
         <v>75</v>
       </c>
       <c r="T104" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="U104" t="n">
         <v>0.1</v>
@@ -12105,7 +12098,7 @@
         <v>75</v>
       </c>
       <c r="W104" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="X104" t="n">
         <v>0.1</v>
@@ -12114,7 +12107,7 @@
         <v>75</v>
       </c>
       <c r="Z104" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AA104" t="n">
         <v>0.1</v>
@@ -12123,7 +12116,7 @@
         <v>75</v>
       </c>
       <c r="AC104" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AD104" t="n">
         <v>0.1</v>
@@ -12132,15 +12125,15 @@
         <v>75</v>
       </c>
       <c r="AF104" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B105" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C105" t="n">
         <v>0.1</v>
@@ -12149,7 +12142,7 @@
         <v>75</v>
       </c>
       <c r="E105" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F105" t="n">
         <v>0.1</v>
@@ -12158,7 +12151,7 @@
         <v>75</v>
       </c>
       <c r="H105" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I105" t="n">
         <v>0.1</v>
@@ -12167,7 +12160,7 @@
         <v>75</v>
       </c>
       <c r="K105" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L105" t="n">
         <v>0.1</v>
@@ -12176,7 +12169,7 @@
         <v>75</v>
       </c>
       <c r="N105" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O105" t="n">
         <v>0.1</v>
@@ -12185,7 +12178,7 @@
         <v>75</v>
       </c>
       <c r="Q105" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="R105" t="n">
         <v>0.1</v>
@@ -12194,7 +12187,7 @@
         <v>75</v>
       </c>
       <c r="T105" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="U105" t="n">
         <v>0.1</v>
@@ -12203,7 +12196,7 @@
         <v>75</v>
       </c>
       <c r="W105" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="X105" t="n">
         <v>0.1</v>
@@ -12212,7 +12205,7 @@
         <v>75</v>
       </c>
       <c r="Z105" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AA105" t="n">
         <v>0.1</v>
@@ -12221,7 +12214,7 @@
         <v>75</v>
       </c>
       <c r="AC105" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AD105" t="n">
         <v>0.1</v>
@@ -12230,15 +12223,15 @@
         <v>75</v>
       </c>
       <c r="AF105" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B106" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C106" t="n">
         <v>0.2</v>
@@ -12274,7 +12267,7 @@
         <v>85</v>
       </c>
       <c r="N106" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="O106" t="n">
         <v>0.1</v>
@@ -12283,7 +12276,7 @@
         <v>85</v>
       </c>
       <c r="Q106" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="R106" t="n">
         <v>0.1</v>
@@ -12292,7 +12285,7 @@
         <v>75</v>
       </c>
       <c r="T106" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="U106" t="n">
         <v>0.1</v>
@@ -12301,7 +12294,7 @@
         <v>75</v>
       </c>
       <c r="W106" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="X106" t="n">
         <v>0.1</v>
@@ -12310,7 +12303,7 @@
         <v>75</v>
       </c>
       <c r="Z106" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AA106" t="n">
         <v>0.1</v>
@@ -12319,7 +12312,7 @@
         <v>75</v>
       </c>
       <c r="AC106" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AD106" t="n">
         <v>0.1</v>
@@ -12328,15 +12321,15 @@
         <v>75</v>
       </c>
       <c r="AF106" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B107" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C107" t="n">
         <v>0</v>
@@ -12345,7 +12338,7 @@
         <v>75</v>
       </c>
       <c r="E107" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
@@ -12354,7 +12347,7 @@
         <v>75</v>
       </c>
       <c r="H107" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I107" t="n">
         <v>0</v>
@@ -12363,7 +12356,7 @@
         <v>75</v>
       </c>
       <c r="K107" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="L107" t="n">
         <v>0.1</v>
@@ -12390,7 +12383,7 @@
         <v>75</v>
       </c>
       <c r="T107" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="U107" t="n">
         <v>0.1</v>
@@ -12399,7 +12392,7 @@
         <v>75</v>
       </c>
       <c r="W107" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="X107" t="n">
         <v>0.1</v>
@@ -12431,10 +12424,10 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B108" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C108" t="n">
         <v>0.1</v>
@@ -12470,7 +12463,7 @@
         <v>75</v>
       </c>
       <c r="N108" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="O108" t="n">
         <v>0</v>
@@ -12479,7 +12472,7 @@
         <v>75</v>
       </c>
       <c r="Q108" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="R108" t="n">
         <v>-0.1</v>
@@ -12488,7 +12481,7 @@
         <v>65</v>
       </c>
       <c r="T108" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="U108" t="n">
         <v>-0.1</v>
@@ -12497,7 +12490,7 @@
         <v>65</v>
       </c>
       <c r="W108" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="X108" t="n">
         <v>0</v>
@@ -12506,7 +12499,7 @@
         <v>75</v>
       </c>
       <c r="Z108" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AA108" t="n">
         <v>0</v>
@@ -12515,7 +12508,7 @@
         <v>75</v>
       </c>
       <c r="AC108" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AD108" t="n">
         <v>0</v>
@@ -12524,15 +12517,15 @@
         <v>75</v>
       </c>
       <c r="AF108" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B109" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C109" t="n">
         <v>0.1</v>
@@ -12541,7 +12534,7 @@
         <v>70</v>
       </c>
       <c r="E109" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F109" t="n">
         <v>0.1</v>
@@ -12550,7 +12543,7 @@
         <v>70</v>
       </c>
       <c r="H109" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I109" t="n">
         <v>0.1</v>
@@ -12559,7 +12552,7 @@
         <v>70</v>
       </c>
       <c r="K109" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L109" t="n">
         <v>0.1</v>
@@ -12586,7 +12579,7 @@
         <v>85</v>
       </c>
       <c r="T109" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="U109" t="n">
         <v>0.1</v>
@@ -12595,7 +12588,7 @@
         <v>85</v>
       </c>
       <c r="W109" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="X109" t="n">
         <v>0.1</v>
@@ -12627,10 +12620,10 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B110" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C110" t="n">
         <v>0.1</v>
@@ -12725,10 +12718,10 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B111" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C111" t="n">
         <v>0.2</v>
@@ -12823,10 +12816,10 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B112" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C112" t="n">
         <v>0.1</v>
@@ -12835,7 +12828,7 @@
         <v>75</v>
       </c>
       <c r="E112" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F112" t="n">
         <v>0.1</v>
@@ -12844,7 +12837,7 @@
         <v>75</v>
       </c>
       <c r="H112" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I112" t="n">
         <v>0.1</v>
@@ -12853,7 +12846,7 @@
         <v>75</v>
       </c>
       <c r="K112" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L112" t="n">
         <v>0.2</v>
@@ -12921,10 +12914,10 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B113" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C113" t="n">
         <v>0.1</v>
@@ -12978,7 +12971,7 @@
         <v>70</v>
       </c>
       <c r="T113" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="U113" t="n">
         <v>0.1</v>
@@ -12987,7 +12980,7 @@
         <v>70</v>
       </c>
       <c r="W113" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="X113" t="n">
         <v>0.1</v>
@@ -13019,10 +13012,10 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B114" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C114" t="n">
         <v>0.1</v>
@@ -13058,7 +13051,7 @@
         <v>75</v>
       </c>
       <c r="N114" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O114" t="n">
         <v>0.1</v>
@@ -13067,7 +13060,7 @@
         <v>75</v>
       </c>
       <c r="Q114" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="R114" t="n">
         <v>0.1</v>
@@ -13076,7 +13069,7 @@
         <v>70</v>
       </c>
       <c r="T114" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="U114" t="n">
         <v>0.1</v>
@@ -13085,7 +13078,7 @@
         <v>70</v>
       </c>
       <c r="W114" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="X114" t="n">
         <v>0.1</v>
@@ -13094,7 +13087,7 @@
         <v>75</v>
       </c>
       <c r="Z114" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AA114" t="n">
         <v>0.1</v>
@@ -13103,7 +13096,7 @@
         <v>75</v>
       </c>
       <c r="AC114" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AD114" t="n">
         <v>0.1</v>
@@ -13112,15 +13105,15 @@
         <v>75</v>
       </c>
       <c r="AF114" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B115" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C115" t="n">
         <v>0.1</v>
@@ -13129,7 +13122,7 @@
         <v>75</v>
       </c>
       <c r="E115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F115" t="n">
         <v>0.1</v>
@@ -13138,7 +13131,7 @@
         <v>75</v>
       </c>
       <c r="H115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I115" t="n">
         <v>0.1</v>
@@ -13147,7 +13140,7 @@
         <v>75</v>
       </c>
       <c r="K115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L115" t="n">
         <v>0.1</v>
@@ -13156,7 +13149,7 @@
         <v>75</v>
       </c>
       <c r="N115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O115" t="n">
         <v>0.1</v>
@@ -13165,7 +13158,7 @@
         <v>75</v>
       </c>
       <c r="Q115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="R115" t="n">
         <v>0.1</v>
@@ -13174,7 +13167,7 @@
         <v>75</v>
       </c>
       <c r="T115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="U115" t="n">
         <v>0.1</v>
@@ -13183,7 +13176,7 @@
         <v>75</v>
       </c>
       <c r="W115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="X115" t="n">
         <v>0.1</v>
@@ -13192,7 +13185,7 @@
         <v>75</v>
       </c>
       <c r="Z115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AA115" t="n">
         <v>0.1</v>
@@ -13201,7 +13194,7 @@
         <v>75</v>
       </c>
       <c r="AC115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AD115" t="n">
         <v>0.1</v>
@@ -13210,15 +13203,15 @@
         <v>75</v>
       </c>
       <c r="AF115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B116" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C116" t="n">
         <v>0.1</v>
@@ -13313,10 +13306,10 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B117" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C117" t="n">
         <v>0.1</v>
@@ -13325,7 +13318,7 @@
         <v>70</v>
       </c>
       <c r="E117" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F117" t="n">
         <v>0.1</v>
@@ -13334,7 +13327,7 @@
         <v>70</v>
       </c>
       <c r="H117" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I117" t="n">
         <v>0.1</v>
@@ -13343,7 +13336,7 @@
         <v>70</v>
       </c>
       <c r="K117" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L117" t="n">
         <v>0.2</v>
@@ -13370,7 +13363,7 @@
         <v>70</v>
       </c>
       <c r="T117" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="U117" t="n">
         <v>0.1</v>
@@ -13379,7 +13372,7 @@
         <v>70</v>
       </c>
       <c r="W117" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="X117" t="n">
         <v>0.2</v>
@@ -13411,10 +13404,10 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B118" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C118" t="n">
         <v>0.1</v>
@@ -13423,7 +13416,7 @@
         <v>75</v>
       </c>
       <c r="E118" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F118" t="n">
         <v>0.1</v>
@@ -13432,7 +13425,7 @@
         <v>75</v>
       </c>
       <c r="H118" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I118" t="n">
         <v>0.1</v>
@@ -13441,7 +13434,7 @@
         <v>75</v>
       </c>
       <c r="K118" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L118" t="n">
         <v>0.2</v>
@@ -13509,10 +13502,10 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B119" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C119" t="n">
         <v>-0.1</v>
@@ -13521,7 +13514,7 @@
         <v>70</v>
       </c>
       <c r="E119" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F119" t="n">
         <v>-0.1</v>
@@ -13530,7 +13523,7 @@
         <v>70</v>
       </c>
       <c r="H119" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I119" t="n">
         <v>-0.1</v>
@@ -13539,7 +13532,7 @@
         <v>70</v>
       </c>
       <c r="K119" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L119" t="n">
         <v>-0.1</v>
@@ -13548,7 +13541,7 @@
         <v>60</v>
       </c>
       <c r="N119" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="O119" t="n">
         <v>-0.1</v>
@@ -13557,7 +13550,7 @@
         <v>60</v>
       </c>
       <c r="Q119" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="R119" t="n">
         <v>0</v>
@@ -13566,7 +13559,7 @@
         <v>70</v>
       </c>
       <c r="T119" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="U119" t="n">
         <v>0</v>
@@ -13575,7 +13568,7 @@
         <v>70</v>
       </c>
       <c r="W119" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="X119" t="n">
         <v>-0.1</v>
@@ -13584,7 +13577,7 @@
         <v>75</v>
       </c>
       <c r="Z119" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AA119" t="n">
         <v>-0.1</v>
@@ -13593,7 +13586,7 @@
         <v>75</v>
       </c>
       <c r="AC119" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AD119" t="n">
         <v>-0.1</v>
@@ -13602,15 +13595,15 @@
         <v>75</v>
       </c>
       <c r="AF119" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B120" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C120" t="n">
         <v>0.1</v>
@@ -13646,7 +13639,7 @@
         <v>70</v>
       </c>
       <c r="N120" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O120" t="n">
         <v>0.1</v>
@@ -13655,7 +13648,7 @@
         <v>70</v>
       </c>
       <c r="Q120" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R120" t="n">
         <v>0.1</v>
@@ -13664,7 +13657,7 @@
         <v>75</v>
       </c>
       <c r="T120" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="U120" t="n">
         <v>0.1</v>
@@ -13673,7 +13666,7 @@
         <v>75</v>
       </c>
       <c r="W120" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="X120" t="n">
         <v>0.1</v>
@@ -13682,7 +13675,7 @@
         <v>75</v>
       </c>
       <c r="Z120" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AA120" t="n">
         <v>0.1</v>
@@ -13691,7 +13684,7 @@
         <v>75</v>
       </c>
       <c r="AC120" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AD120" t="n">
         <v>0.1</v>
@@ -13700,15 +13693,15 @@
         <v>75</v>
       </c>
       <c r="AF120" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B121" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C121" t="n">
         <v>0.1</v>
@@ -13744,7 +13737,7 @@
         <v>75</v>
       </c>
       <c r="N121" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="O121" t="n">
         <v>-0.1</v>
@@ -13753,7 +13746,7 @@
         <v>75</v>
       </c>
       <c r="Q121" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="R121" t="n">
         <v>-0.1</v>
@@ -13762,7 +13755,7 @@
         <v>85</v>
       </c>
       <c r="T121" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="U121" t="n">
         <v>-0.1</v>
@@ -13771,7 +13764,7 @@
         <v>85</v>
       </c>
       <c r="W121" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="X121" t="n">
         <v>-0.1</v>
@@ -13780,7 +13773,7 @@
         <v>75</v>
       </c>
       <c r="Z121" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AA121" t="n">
         <v>-0.1</v>
@@ -13789,7 +13782,7 @@
         <v>75</v>
       </c>
       <c r="AC121" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AD121" t="n">
         <v>-0.1</v>
@@ -13798,15 +13791,15 @@
         <v>75</v>
       </c>
       <c r="AF121" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B122" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C122" t="n">
         <v>0.1</v>
@@ -13901,10 +13894,10 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B123" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C123" t="n">
         <v>0.2</v>
@@ -13940,7 +13933,7 @@
         <v>80</v>
       </c>
       <c r="N123" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="O123" t="n">
         <v>0.1</v>
@@ -13949,7 +13942,7 @@
         <v>80</v>
       </c>
       <c r="Q123" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="R123" t="n">
         <v>0.1</v>
@@ -13999,10 +13992,10 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B124" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C124" t="n">
         <v>0.2</v>
@@ -14038,7 +14031,7 @@
         <v>75</v>
       </c>
       <c r="N124" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="O124" t="n">
         <v>0.2</v>
@@ -14097,10 +14090,10 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B125" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C125" t="n">
         <v>-0.1</v>
@@ -14109,7 +14102,7 @@
         <v>70</v>
       </c>
       <c r="E125" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F125" t="n">
         <v>-0.1</v>
@@ -14118,7 +14111,7 @@
         <v>70</v>
       </c>
       <c r="H125" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I125" t="n">
         <v>-0.1</v>
@@ -14127,7 +14120,7 @@
         <v>70</v>
       </c>
       <c r="K125" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L125" t="n">
         <v>-0.1</v>
@@ -14136,7 +14129,7 @@
         <v>75</v>
       </c>
       <c r="N125" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="O125" t="n">
         <v>-0.1</v>
@@ -14145,7 +14138,7 @@
         <v>75</v>
       </c>
       <c r="Q125" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="R125" t="n">
         <v>-0.1</v>
@@ -14154,7 +14147,7 @@
         <v>70</v>
       </c>
       <c r="T125" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="U125" t="n">
         <v>-0.1</v>
@@ -14163,7 +14156,7 @@
         <v>70</v>
       </c>
       <c r="W125" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="X125" t="n">
         <v>-0.2</v>
@@ -14172,7 +14165,7 @@
         <v>65</v>
       </c>
       <c r="Z125" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="AA125" t="n">
         <v>-0.2</v>
@@ -14181,7 +14174,7 @@
         <v>65</v>
       </c>
       <c r="AC125" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="AD125" t="n">
         <v>-0.2</v>
@@ -14190,15 +14183,15 @@
         <v>65</v>
       </c>
       <c r="AF125" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B126" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C126" t="n">
         <v>0</v>
@@ -14207,7 +14200,7 @@
         <v>65</v>
       </c>
       <c r="E126" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F126" t="n">
         <v>0</v>
@@ -14216,7 +14209,7 @@
         <v>65</v>
       </c>
       <c r="H126" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I126" t="n">
         <v>0</v>
@@ -14225,7 +14218,7 @@
         <v>65</v>
       </c>
       <c r="K126" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="L126" t="n">
         <v>0.1</v>
@@ -14234,7 +14227,7 @@
         <v>70</v>
       </c>
       <c r="N126" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O126" t="n">
         <v>0.1</v>
@@ -14243,7 +14236,7 @@
         <v>70</v>
       </c>
       <c r="Q126" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R126" t="n">
         <v>-0.1</v>
@@ -14252,7 +14245,7 @@
         <v>65</v>
       </c>
       <c r="T126" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="U126" t="n">
         <v>-0.1</v>
@@ -14261,7 +14254,7 @@
         <v>65</v>
       </c>
       <c r="W126" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="X126" t="n">
         <v>-0.1</v>
@@ -14270,7 +14263,7 @@
         <v>65</v>
       </c>
       <c r="Z126" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AA126" t="n">
         <v>-0.1</v>
@@ -14279,7 +14272,7 @@
         <v>65</v>
       </c>
       <c r="AC126" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AD126" t="n">
         <v>-0.1</v>
@@ -14288,15 +14281,15 @@
         <v>65</v>
       </c>
       <c r="AF126" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B127" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C127" t="n">
         <v>0.1</v>
@@ -14305,7 +14298,7 @@
         <v>75</v>
       </c>
       <c r="E127" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F127" t="n">
         <v>0.1</v>
@@ -14314,7 +14307,7 @@
         <v>75</v>
       </c>
       <c r="H127" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I127" t="n">
         <v>0.1</v>
@@ -14323,7 +14316,7 @@
         <v>75</v>
       </c>
       <c r="K127" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L127" t="n">
         <v>0.2</v>
@@ -14391,10 +14384,10 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B128" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C128" t="n">
         <v>0.1</v>
@@ -14489,10 +14482,10 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B129" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C129" t="n">
         <v>0.3</v>
@@ -14564,7 +14557,7 @@
         <v>70</v>
       </c>
       <c r="Z129" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AA129" t="n">
         <v>0.1</v>
@@ -14573,7 +14566,7 @@
         <v>70</v>
       </c>
       <c r="AC129" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AD129" t="n">
         <v>0.1</v>
@@ -14582,15 +14575,15 @@
         <v>70</v>
       </c>
       <c r="AF129" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B130" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C130" t="n">
         <v>0.3</v>
@@ -14685,10 +14678,10 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B131" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C131" t="n">
         <v>0.2</v>
@@ -14697,7 +14690,7 @@
         <v>75</v>
       </c>
       <c r="E131" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F131" t="n">
         <v>0.2</v>
@@ -14760,7 +14753,7 @@
         <v>70</v>
       </c>
       <c r="Z131" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="AA131" t="n">
         <v>-0.1</v>
@@ -14769,7 +14762,7 @@
         <v>70</v>
       </c>
       <c r="AC131" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="AD131" t="n">
         <v>-0.1</v>
@@ -14778,7 +14771,7 @@
         <v>70</v>
       </c>
       <c r="AF131" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>